<commit_message>
Complete overhaul of data pull and plots
</commit_message>
<xml_diff>
--- a/assets/data_sources.xlsx
+++ b/assets/data_sources.xlsx
@@ -5,33 +5,46 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Academic\wiiw_projects\dashboarddb\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiny.cucumber\projects\dashboarddb\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3682D7E-9F76-4393-BF8B-522FBCC400AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18C9226-A709-4D39-BDFB-CBD047D433AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5484" yWindow="2244" windowWidth="16440" windowHeight="9372" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
-    <sheet name="labels_consolidated_budget_rev" sheetId="2" r:id="rId2"/>
-    <sheet name="labels_consolidated_budget_exp" sheetId="3" r:id="rId3"/>
-    <sheet name="labels_consolidated_budget_fin" sheetId="4" r:id="rId4"/>
-    <sheet name="labels_cpi" sheetId="5" r:id="rId5"/>
-    <sheet name="labels_reserves" sheetId="6" r:id="rId6"/>
+    <sheet name="labels_fiscal_income" sheetId="2" r:id="rId2"/>
+    <sheet name="labels_fiscal_expenses" sheetId="3" r:id="rId3"/>
+    <sheet name="labels_fiscal_finance" sheetId="4" r:id="rId4"/>
+    <sheet name="labels_cpi_headline" sheetId="5" r:id="rId5"/>
+    <sheet name="labels_international_reserves" sheetId="6" r:id="rId6"/>
     <sheet name="labels_bond_yields" sheetId="7" r:id="rId7"/>
+    <sheet name="labels_policy_rate" sheetId="8" r:id="rId8"/>
+    <sheet name="labels_interest_rates" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="220">
   <si>
     <t>source</t>
   </si>
@@ -207,9 +220,6 @@
     <t>financial_soundness</t>
   </si>
   <si>
-    <t>2019-2022</t>
-  </si>
-  <si>
     <t>policy_rate</t>
   </si>
   <si>
@@ -321,9 +331,6 @@
     <t>Targeted  funds</t>
   </si>
   <si>
-    <t>budget classification code</t>
-  </si>
-  <si>
     <t>State administration</t>
   </si>
   <si>
@@ -622,16 +629,94 @@
   </si>
   <si>
     <t>EUR: 3 to 5 years: amount</t>
+  </si>
+  <si>
+    <t>column_name</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>sheet_count</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>on a quantitative liquidity-providing tender : maturity: days</t>
+  </si>
+  <si>
+    <t>On a tender on allocation of NBU certificates of deposit : maturity: days</t>
+  </si>
+  <si>
+    <t>on overnight loans: unsecured (blank): % per annum</t>
+  </si>
+  <si>
+    <t>on a quantitative liquidity-providing tender : interest rate: %  per annum</t>
+  </si>
+  <si>
+    <t>on a quantitative liquidity-providing tender : Amount announced : UAH million</t>
+  </si>
+  <si>
+    <t>On a tender on allocation of NBU certificates of deposit : interest rate (maximum): % per annum</t>
+  </si>
+  <si>
+    <t>On a tender on allocation of NBU certificates of deposit : Amount announced : UAH million</t>
+  </si>
+  <si>
+    <t>Reference rate</t>
+  </si>
+  <si>
+    <t>ON deposit rate</t>
+  </si>
+  <si>
+    <t>ON lending rate (collateral)</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nationals: other financial corporations </t>
+  </si>
+  <si>
+    <t>Nationals: general government</t>
+  </si>
+  <si>
+    <t>Nationals: non-financial corporations</t>
+  </si>
+  <si>
+    <t>Nationals: households</t>
+  </si>
+  <si>
+    <t>Nationals: non-profit institutions serving households</t>
+  </si>
+  <si>
+    <t>Nationals: Foreign non-FI</t>
+  </si>
+  <si>
+    <t>Nationals: average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-* #,##0\ _г_р_н_._-;\-* #,##0\ _г_р_н_._-;_-* &quot;-&quot;\ _г_р_н_._-;_-@_-"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ _г_р_н_._-;\-* #,##0\ _г_р_н_._-;_-* &quot;-&quot;\ _г_р_н_._-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _г_р_н_._-;\-* #,##0.00\ _г_р_н_._-;_-* &quot;-&quot;??\ _г_р_н_._-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_г_р_н_._-;\-* #,##0.00_г_р_н_._-;_-* &quot;-&quot;??_г_р_н_._-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="#,##0&quot; р.&quot;;[Red]\-#,##0&quot; р.&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,6 +741,41 @@
       <name val="Arial Cyr"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -674,23 +794,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="38" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="14">
+    <cellStyle name="Comma [0] 2" xfId="9" xr:uid="{68B54856-B8DC-441F-9632-EA7505A3876E}"/>
+    <cellStyle name="Comma 2" xfId="7" xr:uid="{5F0DA3B7-792E-4F84-B341-B1A3C3F3955C}"/>
+    <cellStyle name="Currency [0] 2" xfId="10" xr:uid="{F8990DF4-D14B-4BD5-8A0E-27FC2FF459E0}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="11" xr:uid="{6B101DA7-533C-48EA-A754-69F6149B74AF}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{5846D16B-00CE-4302-8ACA-A32DD5430A29}"/>
-    <cellStyle name="Обычный_Доходнисть ОВДП по м_сяцях" xfId="3" xr:uid="{1361AEF6-690F-4D37-A64B-93AA63877ED3}"/>
-    <cellStyle name="Финансовый [0]_ОВДП_andrej" xfId="4" xr:uid="{05644ADD-A7D0-4C18-AFED-15A2D1B5A10E}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{6EF38448-5EB0-40F9-882E-ADE06D02BAF9}"/>
+    <cellStyle name="Normal 4" xfId="8" xr:uid="{B107585B-A2BA-4B04-8468-7766850C40ED}"/>
+    <cellStyle name="Обычный 2" xfId="5" xr:uid="{B8521A00-FD81-489A-ADB5-E1FBD91C6512}"/>
+    <cellStyle name="Обычный 2 2" xfId="12" xr:uid="{A00752CB-8567-4D0B-B99A-9C392B95C47B}"/>
+    <cellStyle name="Обычный_3.3-Loans" xfId="13" xr:uid="{1EECB0D0-DC8F-4429-9A81-B02F3E9EC8E1}"/>
+    <cellStyle name="Финансовый [0]_ОВДП_andrej" xfId="3" xr:uid="{05644ADD-A7D0-4C18-AFED-15A2D1B5A10E}"/>
+    <cellStyle name="Финансовый 2" xfId="6" xr:uid="{71D0A33E-B46F-4E05-8A79-4D931A7B19DD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -968,20 +1109,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="33.140625" customWidth="1"/>
-    <col min="5" max="5" width="103.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="33.109375" customWidth="1"/>
+    <col min="5" max="5" width="103.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1003,8 +1144,11 @@
       <c r="G1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1015,7 +1159,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -1024,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1044,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1064,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1084,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1104,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1124,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1144,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1164,7 +1308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1187,7 +1331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1210,7 +1354,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1233,7 +1377,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1256,7 +1400,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1279,7 +1423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1290,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>46</v>
@@ -1302,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1313,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>46</v>
@@ -1325,7 +1469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1336,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>46</v>
@@ -1348,7 +1492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1371,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1391,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1410,11 +1554,11 @@
       <c r="F20">
         <v>6</v>
       </c>
-      <c r="G20">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1436,8 +1580,11 @@
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1456,11 +1603,11 @@
       <c r="F22">
         <v>3</v>
       </c>
-      <c r="G22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1471,19 +1618,19 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F23">
-        <v>3</v>
-      </c>
-      <c r="G23">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1494,19 +1641,19 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24">
         <v>3</v>
       </c>
-      <c r="G24">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1517,16 +1664,16 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
-      <c r="G25">
-        <v>2022</v>
+      <c r="H25">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -1545,6 +1692,7 @@
     <hyperlink ref="E22" r:id="rId12" xr:uid="{864CD154-F73E-4563-B7B3-4902C4F5B214}"/>
     <hyperlink ref="E20" r:id="rId13" xr:uid="{A0042D51-75FF-4622-92B3-F85244BF1565}"/>
     <hyperlink ref="E21" r:id="rId14" xr:uid="{34D6EFF7-F5DE-4487-A837-7043BEBA7731}"/>
+    <hyperlink ref="E15" r:id="rId15" xr:uid="{CB2ABF31-9EE8-4678-BF7F-C2E399CDD67F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1552,257 +1700,460 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC56B33F-EF9E-43A0-B1C8-80B283EAD1FB}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="116.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>10000000</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>66</v>
       </c>
-      <c r="B2">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B4">
+        <v>11000000</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>67</v>
       </c>
-      <c r="B3">
-        <v>11000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>11010000</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>68</v>
       </c>
-      <c r="B4">
-        <v>11010000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>11020000</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>69</v>
       </c>
-      <c r="B5">
-        <v>11020000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B7">
+        <v>13000000</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>70</v>
       </c>
-      <c r="B6">
-        <v>13000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B8">
+        <v>13030000</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>71</v>
       </c>
-      <c r="B7">
-        <v>13030000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B9">
+        <v>14000000</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>72</v>
       </c>
-      <c r="B8">
-        <v>14000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="B10">
+        <v>14020000</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>73</v>
       </c>
-      <c r="B9">
-        <v>14020000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="B11">
+        <v>14030000</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
         <v>74</v>
       </c>
-      <c r="B10">
-        <v>14030000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B12">
+        <v>14060000</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>75</v>
       </c>
-      <c r="B11">
-        <v>14060000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="B13">
+        <v>14070000</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>76</v>
       </c>
-      <c r="B12">
-        <v>14070000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="B14">
+        <v>18000000</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>77</v>
       </c>
-      <c r="B13">
-        <v>18000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="B15">
+        <v>18050000</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>78</v>
       </c>
-      <c r="B14">
-        <v>18050000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="B16">
+        <v>19000000</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>79</v>
       </c>
-      <c r="B15">
-        <v>19000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="B17">
+        <v>19010000</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>80</v>
       </c>
-      <c r="B16">
-        <v>19010000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="B18">
+        <v>19060000</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>81</v>
       </c>
-      <c r="B17">
-        <v>19060000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="B19">
+        <v>20000000</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>82</v>
       </c>
-      <c r="B18">
-        <v>20000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="B20">
+        <v>21000000</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>83</v>
       </c>
-      <c r="B19">
-        <v>21000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="B21">
+        <v>21010000</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>84</v>
       </c>
-      <c r="B20">
-        <v>21010000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="B22">
+        <v>21020000</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>85</v>
       </c>
-      <c r="B21">
-        <v>21020000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+      <c r="B23">
+        <v>22000000</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>86</v>
       </c>
-      <c r="B22">
-        <v>22000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="B24">
+        <v>22010000</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
         <v>87</v>
       </c>
-      <c r="B23">
-        <v>22010000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="B25">
+        <v>22080000</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>88</v>
       </c>
-      <c r="B24">
-        <v>22080000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="B26">
+        <v>22090000</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
         <v>89</v>
       </c>
-      <c r="B25">
-        <v>22090000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="B27">
+        <v>24000000</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
         <v>90</v>
       </c>
-      <c r="B26">
-        <v>24000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+      <c r="B28">
+        <v>24140000</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
         <v>91</v>
       </c>
-      <c r="B27">
-        <v>24140000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+      <c r="B29">
+        <v>25000000</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>92</v>
       </c>
-      <c r="B28">
-        <v>25000000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+      <c r="B30">
+        <v>30000000</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
         <v>93</v>
       </c>
-      <c r="B29">
-        <v>30000000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
+      <c r="B31">
+        <v>42000000</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
         <v>94</v>
       </c>
-      <c r="B30">
-        <v>42000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31">
+      <c r="B32">
         <v>50000000</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1812,195 +2163,353 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513465B3-4C57-4E09-A648-DC80E921D9E1}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>97</v>
       </c>
-      <c r="B1">
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5">
+        <v>400</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6">
+        <v>500</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B7">
+        <v>600</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>101</v>
       </c>
-      <c r="B5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B8">
+        <v>700</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>102</v>
       </c>
-      <c r="B6">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B9">
+        <v>800</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>103</v>
       </c>
-      <c r="B7">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B10">
+        <v>900</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>104</v>
       </c>
-      <c r="B8">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13">
+        <v>180</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>105</v>
       </c>
-      <c r="B9">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>106</v>
       </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+      <c r="B15">
+        <v>2000</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="B16">
+        <v>2100</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>108</v>
       </c>
-      <c r="B14">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+      <c r="B17">
+        <v>2200</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>109</v>
       </c>
-      <c r="B15">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+      <c r="B18">
+        <v>2400</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>110</v>
       </c>
-      <c r="B16">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="B19">
+        <v>2600</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>111</v>
       </c>
-      <c r="B17">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="B20">
+        <v>2700</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>112</v>
       </c>
-      <c r="B18">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="B21">
+        <v>2800</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>113</v>
       </c>
-      <c r="B19">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="B22">
+        <v>3000</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>114</v>
       </c>
-      <c r="B20">
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="B23">
+        <v>3100</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>115</v>
       </c>
-      <c r="B21">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23">
+      <c r="B24">
         <v>3200</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>107</v>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2010,243 +2519,448 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FBB677-25A5-40D2-9887-B5212FAAC09C}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D32" sqref="D3:D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3">
+        <v>200000</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B4">
+        <v>202000</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>122</v>
       </c>
-      <c r="B2">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B5">
+        <v>203000</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>123</v>
       </c>
-      <c r="B3">
-        <v>202000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B6">
+        <v>204000</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>124</v>
       </c>
-      <c r="B4">
-        <v>203000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B7">
+        <v>205000</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>125</v>
       </c>
-      <c r="B5">
-        <v>204000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B8">
+        <v>206000</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9">
+        <v>207000</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>126</v>
       </c>
-      <c r="B6">
-        <v>205000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B10">
+        <v>208000</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
         <v>127</v>
       </c>
-      <c r="B7">
-        <v>206000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B11">
+        <v>300000</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12">
+        <v>301000</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13">
+        <v>302000</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14">
+        <v>303000</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15">
+        <v>304000</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16">
+        <v>305000</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17">
+        <v>307000</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19">
+        <v>400000</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>135</v>
       </c>
-      <c r="B8">
-        <v>207000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B9">
-        <v>208000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11">
-        <v>301000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12">
-        <v>302000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13">
-        <v>303000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="B20">
+        <v>401000</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21">
+        <v>402000</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>133</v>
       </c>
-      <c r="B14">
-        <v>304000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15">
-        <v>305000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16">
-        <v>307000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B18">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="B22">
+        <v>403000</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23">
+        <v>500000</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>137</v>
       </c>
-      <c r="B19">
-        <v>401000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="B24">
+        <v>600000</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25">
+        <v>601000</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>138</v>
       </c>
-      <c r="B20">
-        <v>402000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>135</v>
-      </c>
-      <c r="B21">
-        <v>403000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B22">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="B26">
+        <v>602000</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
         <v>139</v>
       </c>
-      <c r="B23">
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24">
-        <v>601000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="B27">
+        <v>603000</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>140</v>
       </c>
-      <c r="B25">
-        <v>602000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="B30">
+        <v>4000</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
         <v>141</v>
       </c>
-      <c r="B26">
-        <v>603000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="B28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+      <c r="B31">
+        <v>4110</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
         <v>142</v>
       </c>
-      <c r="B29">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>143</v>
-      </c>
-      <c r="B30">
-        <v>4110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31">
+      <c r="B32">
         <v>4120</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2256,77 +2970,124 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1849A777-C90B-49D5-991B-3A62E71FECCA}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B3" sqref="B3:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>156</v>
+      <c r="B14" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2336,42 +3097,68 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685009DB-C4A3-4488-B488-CA9A84CEAE18}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>162</v>
+      <c r="B7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2381,180 +3168,533 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E1766A6-64A4-4C45-8F8D-ACA7AF33DD96}">
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="40.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>186</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>187</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>189</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>193</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F5FC06-7EF5-4525-BD48-81E4A2E0AF83}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView zoomScale="60" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="165.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
+        <v>201</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
+        <v>209</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>211</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>204</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>202</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>205</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>206</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>210</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>203</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
+        <v>207</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{591E5F52-587D-419F-A27E-3AF6EE242237}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>195</v>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>